<commit_message>
updated changes for multiple column update
</commit_message>
<xml_diff>
--- a/updated_sample.xlsx
+++ b/updated_sample.xlsx
@@ -43919,13 +43919,13 @@
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="55">
-        <f t="array" ref="M19">IFERROR(SUM(IF($A19=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
+        <f t="array" ref="M19">IFERROR(SUM(IF($A19=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
       </c>
       <c r="N19" s="56">
         <f>N44</f>
       </c>
       <c r="O19" s="57">
-        <f>IFERROR(I19/I$32,0)</f>
+        <f>IFERROR(M19/M$32,0)</f>
       </c>
       <c r="P19" s="58"/>
       <c r="Q19" s="59"/>
@@ -44001,7 +44001,7 @@
         <f>N45</f>
       </c>
       <c r="O20" s="69">
-        <f>IFERROR(I20/I$32,0)</f>
+        <f>IFERROR(M20/M$32,0)</f>
       </c>
       <c r="P20" s="58"/>
       <c r="Q20" s="70"/>
@@ -44141,7 +44141,7 @@
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="55">
-        <f t="array" ref="M23">IFERROR(SUM(IF($A23=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
+        <f t="array" ref="M23">IFERROR(SUM(IF($A23=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
         <v>74.96795081967214</v>
       </c>
       <c r="N23" s="56">
@@ -44149,7 +44149,7 @@
         <v>2453.6758282015103</v>
       </c>
       <c r="O23" s="57">
-        <f>IFERROR(I23/I$32,0)</f>
+        <f>IFERROR(M23/M$32,0)</f>
         <v>1</v>
       </c>
       <c r="P23" s="58"/>
@@ -44224,13 +44224,13 @@
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="55">
-        <f t="array" ref="M24">IFERROR(SUM(IF($A24=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
+        <f t="array" ref="M24">IFERROR(SUM(IF($A24=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
       </c>
       <c r="N24" s="53">
         <f>N48</f>
       </c>
       <c r="O24" s="57">
-        <f>IFERROR(I24/I$32,0)</f>
+        <f>IFERROR(M24/M$32,0)</f>
       </c>
       <c r="P24" s="58"/>
       <c r="Q24" s="59"/>
@@ -44310,7 +44310,7 @@
         <v>2453.6758282015103</v>
       </c>
       <c r="O25" s="69">
-        <f>IFERROR(I25/I$32,0)</f>
+        <f>IFERROR(M25/M$32,0)</f>
         <v>1</v>
       </c>
       <c r="P25" s="58"/>
@@ -44455,13 +44455,13 @@
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="55">
-        <f t="array" ref="M28">IFERROR(SUM(IF($A28=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
+        <f t="array" ref="M28">IFERROR(SUM(IF($A28=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
       </c>
       <c r="N28" s="56">
         <f>N51</f>
       </c>
       <c r="O28" s="57">
-        <f>IFERROR(I28/I$32,0)</f>
+        <f>IFERROR(M28/M$32,0)</f>
       </c>
       <c r="P28" s="58"/>
       <c r="Q28" s="59"/>
@@ -44535,13 +44535,13 @@
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="55">
-        <f t="array" ref="M29">IFERROR(SUM(IF($A29=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
+        <f t="array" ref="M29">IFERROR(SUM(IF($A29=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)/M$94,""),""),"")),0)</f>
       </c>
       <c r="N29" s="53">
         <f>N52</f>
       </c>
       <c r="O29" s="57">
-        <f>IFERROR(I29/I$32,0)</f>
+        <f>IFERROR(M29/M$32,0)</f>
       </c>
       <c r="P29" s="58"/>
       <c r="Q29" s="59"/>
@@ -44619,7 +44619,7 @@
         <f>N53</f>
       </c>
       <c r="O30" s="69">
-        <f>IFERROR(I30/I$32,0)</f>
+        <f>IFERROR(M30/M$32,0)</f>
       </c>
       <c r="P30" s="58"/>
       <c r="Q30" s="70"/>
@@ -44733,7 +44733,7 @@
         <v>4927.404321136134</v>
       </c>
       <c r="O32" s="69">
-        <f>IFERROR(I32/I$32,0)</f>
+        <f>IFERROR(M32/M$32,0)</f>
         <v>1</v>
       </c>
       <c r="P32" s="58"/>
@@ -44794,7 +44794,7 @@
       <c r="K33" s="69"/>
       <c r="L33" s="25"/>
       <c r="M33" s="91">
-        <f>IFERROR(M20/J9,0)</f>
+        <f>IFERROR(M20/N9,0)</f>
       </c>
       <c r="N33" s="68"/>
       <c r="O33" s="69"/>
@@ -44844,7 +44844,7 @@
       <c r="K34" s="69"/>
       <c r="L34" s="92"/>
       <c r="M34" s="91">
-        <f>IFERROR(M25/J11,0)</f>
+        <f>IFERROR(M25/N11,0)</f>
       </c>
       <c r="N34" s="69"/>
       <c r="O34" s="69"/>
@@ -44894,7 +44894,7 @@
       <c r="K35" s="69"/>
       <c r="L35" s="92"/>
       <c r="M35" s="91">
-        <f>IFERROR(M30/J14,0)</f>
+        <f>IFERROR(M30/N14,0)</f>
       </c>
       <c r="N35" s="69"/>
       <c r="O35" s="69"/>
@@ -44944,7 +44944,7 @@
       <c r="K36" s="69"/>
       <c r="L36" s="25"/>
       <c r="M36" s="91">
-        <f>IFERROR(M32/J6,0)</f>
+        <f>IFERROR(M32/N6,0)</f>
         <v>0.94896140278066</v>
       </c>
       <c r="N36" s="94"/>
@@ -45180,7 +45180,7 @@
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="112" t="str">
-        <f>K$2</f>
+        <f>O$2</f>
         <v>T12</v>
       </c>
       <c r="N41" s="112" t="s">
@@ -45329,13 +45329,13 @@
       </c>
       <c r="L44" s="25"/>
       <c r="M44" s="134">
-        <f t="array" ref="M44">IFERROR(SUM(IF($A44=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M44">IFERROR(SUM(IF($A44=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N44" s="56">
-        <f>IFERROR((I44/I19)/12,0)</f>
+        <f>IFERROR((M44/M19)/12,0)</f>
       </c>
       <c r="O44" s="57">
-        <f>IFERROR(I44/I$68,0)</f>
+        <f>IFERROR(M44/M$68,0)</f>
       </c>
       <c r="P44" s="58"/>
       <c r="Q44" s="135"/>
@@ -45410,10 +45410,10 @@
         <f>SUM(M44:M44)</f>
       </c>
       <c r="N45" s="142">
-        <f>IFERROR((I45/I20)/12,0)</f>
+        <f>IFERROR((M45/M20)/12,0)</f>
       </c>
       <c r="O45" s="143">
-        <f>IFERROR(I45/I$68,0)</f>
+        <f>IFERROR(M45/M$68,0)</f>
       </c>
       <c r="P45" s="144"/>
       <c r="Q45" s="145"/>
@@ -45523,15 +45523,15 @@
       </c>
       <c r="L47" s="25"/>
       <c r="M47" s="134">
-        <f t="array" ref="M47">IFERROR(SUM(IF($A47=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M47">IFERROR(SUM(IF($A47=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>2207364.5857923497</v>
       </c>
       <c r="N47" s="56">
-        <f>IFERROR((I47/I23)/12,0)</f>
+        <f>IFERROR((M47/M23)/12,0)</f>
         <v>2453.6758282015103</v>
       </c>
       <c r="O47" s="57">
-        <f>IFERROR(I47/I$68,0)</f>
+        <f>IFERROR(M47/M$68,0)</f>
         <v>0.32000521165830675</v>
       </c>
       <c r="P47" s="58"/>
@@ -45606,13 +45606,13 @@
       </c>
       <c r="L48" s="25"/>
       <c r="M48" s="134">
-        <f t="array" ref="M48">IFERROR(SUM(IF($A48=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M48">IFERROR(SUM(IF($A48=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N48" s="56">
-        <f>IFERROR((I48/I24)/12,0)</f>
+        <f>IFERROR((M48/M24)/12,0)</f>
       </c>
       <c r="O48" s="57">
-        <f>IFERROR(I48/I$68,0)</f>
+        <f>IFERROR(M48/M$68,0)</f>
       </c>
       <c r="P48" s="58"/>
       <c r="Q48" s="135"/>
@@ -45684,11 +45684,11 @@
         <v>2207364.5857923497</v>
       </c>
       <c r="N49" s="142">
-        <f>IFERROR((I49/I25)/12,0)</f>
+        <f>IFERROR((M49/M25)/12,0)</f>
         <v>2453.6758282015103</v>
       </c>
       <c r="O49" s="143">
-        <f>IFERROR(I49/I$68,0)</f>
+        <f>IFERROR(M49/M$68,0)</f>
         <v>0.32000521165830675</v>
       </c>
       <c r="P49" s="144"/>
@@ -45792,14 +45792,14 @@
       </c>
       <c r="L51" s="25"/>
       <c r="M51" s="134">
-        <f t="array" ref="M51">IFERROR(SUM(IF($A51=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M51">IFERROR(SUM(IF($A51=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>2232651.995218579</v>
       </c>
       <c r="N51" s="56">
-        <f>IFERROR((I51/I28)/12,0)</f>
+        <f>IFERROR((M51/M28)/12,0)</f>
       </c>
       <c r="O51" s="57">
-        <f t="shared" ref="O51:O56" si="2">IFERROR(I51/I$68,0)</f>
+        <f t="shared" ref="O51:O56" si="2">IFERROR(M51/M$68,0)</f>
         <v>0.32367116827363684</v>
       </c>
       <c r="P51" s="58"/>
@@ -45871,10 +45871,10 @@
       </c>
       <c r="L52" s="25"/>
       <c r="M52" s="134">
-        <f t="array" ref="M52">IFERROR(SUM(IF($A52=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M52">IFERROR(SUM(IF($A52=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N52" s="56">
-        <f>IFERROR((I52/I29)/12,0)</f>
+        <f>IFERROR((M52/M29)/12,0)</f>
       </c>
       <c r="O52" s="57">
         <f t="shared" si="2"/>
@@ -45950,7 +45950,7 @@
         <v>2232651.995218579</v>
       </c>
       <c r="N53" s="142">
-        <f>IFERROR((I53/I30)/12,0)</f>
+        <f>IFERROR((M53/M30)/12,0)</f>
       </c>
       <c r="O53" s="143">
         <f t="shared" si="2"/>
@@ -46025,11 +46025,11 @@
       </c>
       <c r="L54" s="25"/>
       <c r="M54" s="133">
-        <f t="array" ref="M54">IFERROR(SUM(IF($A54=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M54">IFERROR(SUM(IF($A54=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>-7247.7232240437115</v>
       </c>
       <c r="N54" s="53">
-        <f>IFERROR((I54/I32)/12,0)</f>
+        <f>IFERROR((M54/M32)/12,0)</f>
         <v>-8.056468513989154</v>
       </c>
       <c r="O54" s="54">
@@ -46105,10 +46105,10 @@
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="133">
-        <f t="array" ref="M55">IFERROR(SUM(IF($A55=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M55">IFERROR(SUM(IF($A55=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N55" s="53">
-        <f>IFERROR((I55/I32)/12,0)</f>
+        <f>IFERROR((M55/M32)/12,0)</f>
       </c>
       <c r="O55" s="54">
         <f t="shared" si="2"/>
@@ -46184,7 +46184,7 @@
         <v>4432768.8577868845</v>
       </c>
       <c r="N56" s="68">
-        <f>IFERROR((I56/I32)/12,0)</f>
+        <f>IFERROR((M56/M32)/12,0)</f>
         <v>4927.404321136134</v>
       </c>
       <c r="O56" s="69">
@@ -46324,15 +46324,15 @@
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="134">
-        <f t="array" ref="M59">IFERROR(SUM(IF($A59=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M59">IFERROR(SUM(IF($A59=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>883813.7325136613</v>
       </c>
       <c r="N59" s="56">
-        <f>IFERROR((I$59/I$25)/12,0)</f>
+        <f>IFERROR((M$59/M$25)/12,0)</f>
         <v>982.4350748668435</v>
       </c>
       <c r="O59" s="57">
-        <f>IFERROR(I59/I$68,0)</f>
+        <f>IFERROR(M59/M$68,0)</f>
         <v>0.12812790526764303</v>
       </c>
       <c r="P59" s="58"/>
@@ -46404,14 +46404,14 @@
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="134">
-        <f t="array" ref="M60">IFERROR(SUM(IF($A60=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M60">IFERROR(SUM(IF($A60=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>1311057.4019125686</v>
       </c>
       <c r="N60" s="56">
-        <f>IFERROR((I$60/I$30)/12,0)</f>
+        <f>IFERROR((M$60/M$30)/12,0)</f>
       </c>
       <c r="O60" s="57">
-        <f>IFERROR(I60/I$68,0)</f>
+        <f>IFERROR(M60/M$68,0)</f>
         <v>0.1900661105535597</v>
       </c>
       <c r="P60" s="58"/>
@@ -46483,13 +46483,13 @@
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="134">
-        <f t="array" ref="M61">IFERROR(SUM(IF($A61=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M61">IFERROR(SUM(IF($A61=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N61" s="56">
-        <f>IFERROR((I$61/I$32)/12,0)</f>
+        <f>IFERROR((M$61/M$32)/12,0)</f>
       </c>
       <c r="O61" s="57">
-        <f>IFERROR(I61/I$68,0)</f>
+        <f>IFERROR(M61/M$68,0)</f>
       </c>
       <c r="P61" s="58"/>
       <c r="Q61" s="135"/>
@@ -46560,14 +46560,14 @@
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="134">
-        <f t="array" ref="M62">IFERROR(SUM(IF($A62=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M62">IFERROR(SUM(IF($A62=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>5684.426229508197</v>
       </c>
       <c r="N62" s="56">
-        <f>IFERROR((I$61/I$32)/12,0)</f>
+        <f>IFERROR((M$61/M$32)/12,0)</f>
       </c>
       <c r="O62" s="57">
-        <f>IFERROR(I62/I$68,0)</f>
+        <f>IFERROR(M62/M$68,0)</f>
         <v>0.0008240804579533659</v>
       </c>
       <c r="P62" s="58"/>
@@ -46639,11 +46639,11 @@
         <v>2200555.5606557378</v>
       </c>
       <c r="N63" s="68">
-        <f>IFERROR((I$63/I$32)/12,0)</f>
+        <f>IFERROR((M$63/M$32)/12,0)</f>
         <v>2446.107010390961</v>
       </c>
       <c r="O63" s="69">
-        <f>IFERROR(I63/I$68,0)</f>
+        <f>IFERROR(M63/M$68,0)</f>
         <v>0.31901809627915606</v>
       </c>
       <c r="P63" s="164"/>
@@ -46742,15 +46742,15 @@
       </c>
       <c r="L65" s="25"/>
       <c r="M65" s="134">
-        <f t="array" ref="M65">IFERROR(SUM(IF($A65=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M65">IFERROR(SUM(IF($A65=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>267467.2131147541</v>
       </c>
       <c r="N65" s="56">
-        <f>IFERROR((I$65/I$32)/12,0)</f>
+        <f>IFERROR((M$65/M$32)/12,0)</f>
         <v>297.3128407877027</v>
       </c>
       <c r="O65" s="57">
-        <f>IFERROR(I65/I$68,0)</f>
+        <f>IFERROR(M65/M$68,0)</f>
         <v>0.03877515417948996</v>
       </c>
       <c r="P65" s="58"/>
@@ -46820,15 +46820,15 @@
       </c>
       <c r="L66" s="25"/>
       <c r="M66" s="134">
-        <f t="array" ref="M66">IFERROR(SUM(IF($A66=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M66">IFERROR(SUM(IF($A66=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>-2889.6431693989084</v>
       </c>
       <c r="N66" s="56">
-        <f>IFERROR((I$66/I$32)/12,0)</f>
+        <f>IFERROR((M$66/M$32)/12,0)</f>
         <v>-3.212087229503416</v>
       </c>
       <c r="O66" s="57">
-        <f>IFERROR(I66/I$68,0)</f>
+        <f>IFERROR(M66/M$68,0)</f>
         <v>-0.00041891624065743086</v>
       </c>
       <c r="P66" s="58"/>
@@ -46898,13 +46898,13 @@
       </c>
       <c r="L67" s="168"/>
       <c r="M67" s="172">
-        <f t="array" ref="M67">IFERROR(SUM(IF($A67=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M67">IFERROR(SUM(IF($A67=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N67" s="173">
-        <f>IFERROR((I67/$E$32)/12,0)</f>
+        <f>IFERROR((M67/$E$32)/12,0)</f>
       </c>
       <c r="O67" s="174">
-        <f>IFERROR(I67/I$68,0)</f>
+        <f>IFERROR(M67/M$68,0)</f>
       </c>
       <c r="P67" s="175"/>
       <c r="Q67" s="176"/>
@@ -46975,11 +46975,11 @@
         <v>6897901.988387977</v>
       </c>
       <c r="N68" s="184">
-        <f>IFERROR(I68/(I$32*I$96*I$95),0)</f>
+        <f>IFERROR(M68/(M$32*M$96*M$95),0)</f>
         <v>7688.619241482787</v>
       </c>
       <c r="O68" s="185">
-        <f>IFERROR(I68/I$68,0)</f>
+        <f>IFERROR(M68/M$68,0)</f>
         <v>1</v>
       </c>
       <c r="P68" s="186"/>
@@ -47128,7 +47128,7 @@
       </c>
       <c r="L71" s="5"/>
       <c r="M71" s="112" t="str">
-        <f>K$2</f>
+        <f>O$2</f>
         <v>T12</v>
       </c>
       <c r="N71" s="112" t="s">
@@ -47200,13 +47200,13 @@
       </c>
       <c r="L72" s="43"/>
       <c r="M72" s="153">
-        <f t="array" ref="M72">IFERROR(SUM(IF($A72=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M72">IFERROR(SUM(IF($A72=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N72" s="45">
-        <f>IFERROR((I72/I$32)/12,0)</f>
+        <f>IFERROR((M72/M$32)/12,0)</f>
       </c>
       <c r="O72" s="76">
-        <f t="shared" ref="O72:O88" si="7">IFERROR(I72/I$68,0)</f>
+        <f t="shared" ref="O72:O88" si="7">IFERROR(M72/M$68,0)</f>
       </c>
       <c r="P72" s="77"/>
       <c r="Q72" s="154"/>
@@ -47276,11 +47276,11 @@
       </c>
       <c r="L73" s="25"/>
       <c r="M73" s="134">
-        <f t="array" ref="M73">IFERROR(SUM(IF($A73=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M73">IFERROR(SUM(IF($A73=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>721852.7512295085</v>
       </c>
       <c r="N73" s="53">
-        <f>IFERROR((I73/I$32)/12,0)</f>
+        <f>IFERROR((M73/M$32)/12,0)</f>
         <v>802.4014966140361</v>
       </c>
       <c r="O73" s="57">
@@ -47356,11 +47356,11 @@
       </c>
       <c r="L74" s="25"/>
       <c r="M74" s="134">
-        <f t="array" ref="M74">IFERROR(SUM(IF($A74=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M74">IFERROR(SUM(IF($A74=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>259432.80519125692</v>
       </c>
       <c r="N74" s="53">
-        <f t="shared" ref="N74:N87" si="12">IFERROR((I74/I$32)/12,0)</f>
+        <f t="shared" ref="N74:N87" si="12">IFERROR((M74/M$32)/12,0)</f>
         <v>288.38190448353106</v>
       </c>
       <c r="O74" s="57">
@@ -47436,7 +47436,7 @@
       </c>
       <c r="L75" s="25"/>
       <c r="M75" s="134">
-        <f t="array" ref="M75">IFERROR(SUM(IF($A75=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M75">IFERROR(SUM(IF($A75=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>167878.66844262296</v>
       </c>
       <c r="N75" s="53">
@@ -47516,7 +47516,7 @@
       </c>
       <c r="L76" s="25"/>
       <c r="M76" s="134">
-        <f t="array" ref="M76">IFERROR(SUM(IF($A76=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M76">IFERROR(SUM(IF($A76=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
       </c>
       <c r="N76" s="53">
         <f t="shared" si="12"/>
@@ -47593,7 +47593,7 @@
       </c>
       <c r="L77" s="25"/>
       <c r="M77" s="134">
-        <f t="array" ref="M77">IFERROR(SUM(IF($A77=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M77">IFERROR(SUM(IF($A77=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>832809.9887978147</v>
       </c>
       <c r="N77" s="53">
@@ -47673,7 +47673,7 @@
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="134">
-        <f t="array" ref="M78">IFERROR(SUM(IF($A78=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M78">IFERROR(SUM(IF($A78=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>417218.6751366125</v>
       </c>
       <c r="N78" s="53">
@@ -47753,7 +47753,7 @@
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="134">
-        <f t="array" ref="M79">IFERROR(SUM(IF($A79=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M79">IFERROR(SUM(IF($A79=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>1400820.0867486345</v>
       </c>
       <c r="N79" s="53">
@@ -47833,7 +47833,7 @@
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="134">
-        <f t="array" ref="M80">IFERROR(SUM(IF($A80=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M80">IFERROR(SUM(IF($A80=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>1562941.4087431694</v>
       </c>
       <c r="N80" s="53">
@@ -47913,7 +47913,7 @@
       </c>
       <c r="L81" s="25"/>
       <c r="M81" s="134">
-        <f t="array" ref="M81">IFERROR(SUM(IF($A81=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M81">IFERROR(SUM(IF($A81=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>4724.097267759564</v>
       </c>
       <c r="N81" s="53">
@@ -47993,7 +47993,7 @@
       </c>
       <c r="L82" s="25"/>
       <c r="M82" s="134">
-        <f t="array" ref="M82">IFERROR(SUM(IF($A82=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M82">IFERROR(SUM(IF($A82=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>238503.17663934428</v>
       </c>
       <c r="N82" s="53">
@@ -48073,7 +48073,7 @@
       </c>
       <c r="L83" s="25"/>
       <c r="M83" s="134">
-        <f t="array" ref="M83">IFERROR(SUM(IF($A83=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M83">IFERROR(SUM(IF($A83=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>59725.737841530055</v>
       </c>
       <c r="N83" s="53">
@@ -48153,7 +48153,7 @@
       </c>
       <c r="L84" s="25"/>
       <c r="M84" s="134">
-        <f t="array" ref="M84">IFERROR(SUM(IF($A84=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M84">IFERROR(SUM(IF($A84=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>209611.02322404357</v>
       </c>
       <c r="N84" s="53">
@@ -48233,7 +48233,7 @@
       </c>
       <c r="L85" s="25"/>
       <c r="M85" s="134">
-        <f t="array" ref="M85">IFERROR(SUM(IF($A85=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M85">IFERROR(SUM(IF($A85=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>273313.78510928963</v>
       </c>
       <c r="N85" s="53">
@@ -48313,7 +48313,7 @@
       </c>
       <c r="L86" s="25"/>
       <c r="M86" s="134">
-        <f t="array" ref="M86">IFERROR(SUM(IF($A86=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M86">IFERROR(SUM(IF($A86=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>20234.114071038253</v>
       </c>
       <c r="N86" s="53">
@@ -48393,7 +48393,7 @@
       </c>
       <c r="L87" s="168"/>
       <c r="M87" s="172">
-        <f t="array" ref="M87">IFERROR(SUM(IF($A87=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(J$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
+        <f t="array" ref="M87">IFERROR(SUM(IF($A87=INDIRECT($B$132),IF(M$2&lt;=INDIRECT($A$132),IF(N$2&gt;=INDIRECT($A$132),INDIRECT($C$132)*M$95,""),""),"")),0)</f>
         <v>426582.50081967213</v>
       </c>
       <c r="N87" s="204">
@@ -48475,7 +48475,7 @@
         <v>6169066.318442626</v>
       </c>
       <c r="N88" s="184">
-        <f>IFERROR(I88/(I$32*I$96*I$95),0)</f>
+        <f>IFERROR(M88/(M$32*M$96*M$95),0)</f>
         <v>6876.236003035179</v>
       </c>
       <c r="O88" s="185">
@@ -48583,11 +48583,11 @@
         <v>728835.6699453508</v>
       </c>
       <c r="N90" s="184">
-        <f>IFERROR(I90/(I$32*I$96*I$95),0)</f>
+        <f>IFERROR(M90/(M$32*M$96*M$95),0)</f>
         <v>812.3832384476085</v>
       </c>
       <c r="O90" s="185">
-        <f t="shared" ref="O90" si="17">IFERROR(I90/I$68,0)</f>
+        <f t="shared" ref="O90" si="17">IFERROR(M90/M$68,0)</f>
         <v>0.10566048505361236</v>
       </c>
       <c r="P90" s="186"/>
@@ -48660,11 +48660,11 @@
         <v>344895.0994193989</v>
       </c>
       <c r="N91" s="56">
-        <f>IFERROR((I91/$I$32)/12,0)</f>
+        <f>IFERROR((M91/$M$32)/12,0)</f>
         <v>383.3806042542647</v>
       </c>
       <c r="O91" s="57">
-        <f>IFERROR(I91/I$68,0)</f>
+        <f>IFERROR(M91/M$68,0)</f>
         <v>0.05</v>
       </c>
       <c r="P91" s="58"/>
@@ -48738,11 +48738,11 @@
         <v>383940.570525952</v>
       </c>
       <c r="N92" s="184">
-        <f>IFERROR(I92/(I$32*I$96*I$95),0)</f>
+        <f>IFERROR(M92/(M$32*M$96*M$95),0)</f>
         <v>427.95227637346915</v>
       </c>
       <c r="O92" s="185">
-        <f>IFERROR(I92/I$68,0)</f>
+        <f>IFERROR(M92/M$68,0)</f>
         <v>0.05566048505361236</v>
       </c>
       <c r="P92" s="186"/>
@@ -48830,7 +48830,7 @@
       <c r="K94" s="225"/>
       <c r="L94" s="5"/>
       <c r="M94" s="229">
-        <f>J$2-M$2+1</f>
+        <f>N$2-M$2+1</f>
         <v>366</v>
       </c>
       <c r="N94" s="225"/>
@@ -48922,7 +48922,7 @@
       <c r="K96" s="225"/>
       <c r="L96" s="5"/>
       <c r="M96" s="229">
-        <f>ROUND((J$2-M$2+15)/30.5,0)</f>
+        <f>ROUND((N$2-M$2+15)/30.5,0)</f>
         <v>12</v>
       </c>
       <c r="N96" s="225"/>
@@ -49093,11 +49093,11 @@
         <v>0.095</v>
       </c>
       <c r="N100" s="238">
-        <f>$I$92/I100</f>
+        <f>$M$92/M100</f>
         <v>4041479.6897468627</v>
       </c>
       <c r="O100" s="238">
-        <f>IFERROR($J100/J$7,0)</f>
+        <f>IFERROR($N100/N$7,0)</f>
         <v>53177.36433877451</v>
       </c>
       <c r="P100" s="239"/>
@@ -49166,11 +49166,11 @@
         <v>0.09</v>
       </c>
       <c r="N101" s="243">
-        <f t="shared" ref="N101:N107" si="26">$I$92/I101</f>
+        <f t="shared" ref="N101:N107" si="26">$M$92/M101</f>
         <v>4266006.339177244</v>
       </c>
       <c r="O101" s="243">
-        <f t="shared" ref="O101:O107" si="27">IFERROR($J101/J$7,0)</f>
+        <f t="shared" ref="O101:O107" si="27">IFERROR($N101/N$7,0)</f>
         <v>56131.66235759532</v>
       </c>
       <c r="P101" s="244"/>
@@ -49702,7 +49702,7 @@
       </c>
       <c r="N111" s="2"/>
       <c r="O111" s="256">
-        <f>I111-J111</f>
+        <f>M111-N111</f>
         <v>6897901.988387977</v>
       </c>
       <c r="Q111" s="255"/>
@@ -49738,7 +49738,7 @@
         <v>99</v>
       </c>
       <c r="O112" s="259">
-        <f>IFERROR(O111/I111,0)</f>
+        <f>IFERROR(O111/M111,0)</f>
         <v>1</v>
       </c>
       <c r="Q112" s="257"/>
@@ -49818,7 +49818,7 @@
       </c>
       <c r="N114" s="2"/>
       <c r="O114" s="256">
-        <f>I114-J114</f>
+        <f>M114-N114</f>
         <v>6595648.819262298</v>
       </c>
       <c r="Q114" s="255"/>
@@ -49854,7 +49854,7 @@
         <v>99</v>
       </c>
       <c r="O115" s="262">
-        <f>IFERROR(O114/I114,0)</f>
+        <f>IFERROR(O114/M114,0)</f>
         <v>1</v>
       </c>
       <c r="Q115" s="260"/>

</xml_diff>